<commit_message>
UIPath Project built to uplaod users to an orchestrator queue. Needs to be published to run every monday after CRUD updates. CRUD functionality ongoing, delete is working while create is in progress. Report collating and number functions begining on 07.07.2020
</commit_message>
<xml_diff>
--- a/Kings Casino User Database/Kings Casino - User Database.xlsx
+++ b/Kings Casino User Database/Kings Casino - User Database.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daryl Atienza\Desktop\RPA\RPA.QA.FINAL PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Work\QA Consulting\Training Notes\Project Final\Kings Casino User Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1D6598-F942-4101-B573-65D479EEE852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D2D73F-029F-4184-B26F-EAF86A22FA20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B2960FA7-55C5-4140-B403-93D9D63BED3A}"/>
+    <workbookView xWindow="7275" yWindow="2820" windowWidth="14820" windowHeight="7500" xr2:uid="{B2960FA7-55C5-4140-B403-93D9D63BED3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -553,7 +550,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +596,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>48534</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -620,8 +620,14 @@
       <c r="H2">
         <v>123</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3483423</v>
+      </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -643,8 +649,14 @@
       <c r="H3">
         <v>123</v>
       </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>486343</v>
+      </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -666,8 +678,14 @@
       <c r="H4">
         <v>123</v>
       </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>153485</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -689,8 +707,14 @@
       <c r="H5">
         <v>123</v>
       </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8646</v>
+      </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -712,8 +736,14 @@
       <c r="H6">
         <v>123</v>
       </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1237485</v>
+      </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -735,8 +765,14 @@
       <c r="H7">
         <v>123</v>
       </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>486</v>
+      </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -758,8 +794,14 @@
       <c r="H8">
         <v>123</v>
       </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8643</v>
+      </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -781,8 +823,14 @@
       <c r="H9">
         <v>123</v>
       </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>34856341</v>
+      </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -804,8 +852,14 @@
       <c r="H10">
         <v>123</v>
       </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>748641</v>
+      </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -826,6 +880,9 @@
       </c>
       <c r="H11">
         <v>123</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>